<commit_message>
Use sample data file from under-test code for generator tests User Story #1090: try-yofi.com: Improve sample data
</commit_message>
<xml_diff>
--- a/YoFi.AspNet/Data/FullSampleDataDefinition.xlsx
+++ b/YoFi.AspNet/Data/FullSampleDataDefinition.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\jcoliz\Ofx\YoFi.AspNet\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6843876-EE72-4198-9841-B8ACB22327B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E237FFF-D9DF-4905-846B-4A8895FE1D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6130" yWindow="3350" windowWidth="28800" windowHeight="15460" xr2:uid="{D78380F0-A539-4D8B-9BEC-B3C0621EF4A6}"/>
+    <workbookView xWindow="10110" yWindow="2730" windowWidth="28800" windowHeight="15460" xr2:uid="{D78380F0-A539-4D8B-9BEC-B3C0621EF4A6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Definition" sheetId="1" r:id="rId1"/>
+    <sheet name="SampleDataPattern" sheetId="1" r:id="rId1"/>
+    <sheet name="Need Want Save" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="9" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="102">
   <si>
     <t>Housing:Mortgage Interest</t>
   </si>
@@ -316,6 +320,30 @@
   </si>
   <si>
     <t>Ralphs</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Need</t>
+  </si>
+  <si>
+    <t>Want</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of AmountYearly</t>
+  </si>
+  <si>
+    <t>Net Pay</t>
   </si>
 </sst>
 </file>
@@ -359,17 +387,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -404,10 +440,1438 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-0F7B-43B9-82D3-21798F94FF3C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-0F7B-43B9-82D3-21798F94FF3C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-0F7B-43B9-82D3-21798F94FF3C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Need Want Save'!$A$11:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Need</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Want</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Save</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Need Want Save'!$B$11:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>56770</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17184</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43174</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0F7B-43B9-82D3-21798F94FF3C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>111125</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>60324</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>50799</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{134810A8-0292-46A5-8944-EF8079CE4A5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="James Coliz" refreshedDate="44475.818932986112" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="45" xr:uid="{979DF2D5-559B-47AA-AEFA-1764B35F70D3}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="Category" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Payee" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="AmountYearly" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="-19000" maxValue="120000"/>
+    </cacheField>
+    <cacheField name="DateFrequency" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="AmountJitter" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="DateJitter" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Group" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Classification" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Need"/>
+        <s v="Want"/>
+        <s v="Paycheck"/>
+        <s v="Save"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="45">
+  <r>
+    <s v="Savings:Mortgage Principal"/>
+    <s v="Chase Bank Mortgage"/>
+    <n v="-9600"/>
+    <s v="Monthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Mortgage"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Housing:Mortgage Interest"/>
+    <m/>
+    <n v="-8400"/>
+    <s v="Monthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Mortgage"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Housing:Condo Fees"/>
+    <s v="Farquat Homeowners Assoc"/>
+    <n v="-3960"/>
+    <s v="Monthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Housing:Insurance"/>
+    <s v="GEICO Homeowners Insurance"/>
+    <n v="-400"/>
+    <s v="Yearly"/>
+    <s v="None"/>
+    <s v="High"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Housing:Property Tax"/>
+    <s v="County of Windsor Assessors Office"/>
+    <n v="-5000"/>
+    <s v="Yearly"/>
+    <s v="None"/>
+    <s v="High"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Housing:Repairs &amp; Maintenance"/>
+    <s v="Connor Construction"/>
+    <n v="-3600"/>
+    <s v="Quarterly"/>
+    <s v="Moderate"/>
+    <s v="High"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Housing:Utilities:Gas"/>
+    <s v="Central Gas Electric"/>
+    <n v="-800"/>
+    <s v="Monthly"/>
+    <s v="Low"/>
+    <s v="None"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Housing:Utilities:Electric"/>
+    <s v="Central Gas Electric"/>
+    <n v="-600"/>
+    <s v="Monthly"/>
+    <s v="Low"/>
+    <s v="None"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Housing:Utilities:Trash"/>
+    <s v="Waste Management"/>
+    <n v="-700"/>
+    <s v="Monthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Housing:Utilities:Water &amp; Sewer"/>
+    <s v="Windsor County Water Co"/>
+    <n v="-400"/>
+    <s v="Monthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Housing:Utilities:Cable TV"/>
+    <s v="Viacom"/>
+    <n v="-1140"/>
+    <s v="Monthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Housing:Utilities:Cellular"/>
+    <s v="Sprint"/>
+    <n v="-480"/>
+    <s v="Monthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Housing:Home Goods"/>
+    <s v="Bed Bath Beyond,Target,Container Store"/>
+    <n v="-2400"/>
+    <s v="Weekly"/>
+    <s v="High"/>
+    <s v="High"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Food:At Home"/>
+    <s v="Ralphs"/>
+    <n v="-4420"/>
+    <s v="Weekly"/>
+    <s v="Moderate"/>
+    <s v="Low"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Food:Away:Coffee"/>
+    <s v="Starbucks,Uptown Espresso,Tim Hortons"/>
+    <n v="-1170"/>
+    <s v="ManyPerWeek"/>
+    <s v="High"/>
+    <s v="High"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Food:Away:Dinner"/>
+    <s v="Applebees,Olive Garden,Spaghetti Factory"/>
+    <n v="-7800"/>
+    <s v="ManyPerWeek"/>
+    <s v="High"/>
+    <s v="High"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Healthcare:Co-Pays"/>
+    <s v="Providence Medical"/>
+    <n v="-400"/>
+    <s v="Quarterly"/>
+    <s v="High"/>
+    <s v="High"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Healthcare:Out-of-pocket"/>
+    <s v="Providence Medical"/>
+    <n v="-1200"/>
+    <s v="Quarterly"/>
+    <s v="High"/>
+    <s v="High"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Personal:Clothing"/>
+    <s v="Nordstrom"/>
+    <n v="-1800"/>
+    <s v="Weekly"/>
+    <s v="High"/>
+    <s v="High"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Personal:Haircuts"/>
+    <s v="Zohan Dvir"/>
+    <n v="-240"/>
+    <s v="Quarterly"/>
+    <s v="None"/>
+    <s v="Moderate"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Personal:Apps"/>
+    <s v="iTunes App Store"/>
+    <n v="-250"/>
+    <s v="Monthly"/>
+    <s v="High"/>
+    <s v="High"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Personal:Electronics"/>
+    <s v="Amazon"/>
+    <n v="-2400"/>
+    <s v="Weekly"/>
+    <s v="High"/>
+    <s v="High"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Transportation:Fuel"/>
+    <s v="Standard Oil"/>
+    <n v="-1820"/>
+    <s v="Weekly"/>
+    <s v="High"/>
+    <s v="Moderate"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Transportation:Insurance"/>
+    <s v="GEICO Auto Insurance"/>
+    <n v="-500"/>
+    <s v="Quarterly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Transportation:Registration"/>
+    <s v="Windsor County DMV"/>
+    <n v="-300"/>
+    <s v="Yearly"/>
+    <s v="Low"/>
+    <s v="None"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Transportation:Car Payment"/>
+    <s v="Chase Bank Auto Loans"/>
+    <n v="-4800"/>
+    <s v="Monthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Transportation:Repairs &amp; Maintenance"/>
+    <s v="Mikes Wrenchems"/>
+    <n v="-2000"/>
+    <s v="Quarterly"/>
+    <s v="High"/>
+    <s v="High"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Entertainment:Disney Plus"/>
+    <s v="Disney Plus"/>
+    <n v="-144"/>
+    <s v="Monthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Entertainment:Netflix"/>
+    <s v="Netflix"/>
+    <n v="-180"/>
+    <s v="Monthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Entertainment:Cinema"/>
+    <s v="AMC"/>
+    <n v="-300"/>
+    <s v="Monthly"/>
+    <s v="Low"/>
+    <s v="High"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Entertainment:Go-Karts"/>
+    <s v="Speedy Speeds"/>
+    <n v="-500"/>
+    <s v="Quarterly"/>
+    <s v="Low"/>
+    <s v="Moderate"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Income:Bonus"/>
+    <s v="Megacorp Inc"/>
+    <n v="25000"/>
+    <s v="Yearly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Income:Salary"/>
+    <s v="Megacorp Inc"/>
+    <n v="120000"/>
+    <s v="SemiMonthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Paycheck"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Income:401k Match"/>
+    <m/>
+    <n v="4000"/>
+    <s v="SemiMonthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Paycheck"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Taxes:Federal:Paycheck"/>
+    <m/>
+    <n v="-16488"/>
+    <s v="SemiMonthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Paycheck"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Taxes:SSA"/>
+    <m/>
+    <n v="-7440"/>
+    <s v="SemiMonthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Paycheck"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Taxes:Medicare"/>
+    <m/>
+    <n v="-1752"/>
+    <s v="SemiMonthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Paycheck"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Taxes:State Income"/>
+    <m/>
+    <n v="-6240"/>
+    <s v="SemiMonthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Paycheck"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Taxes:State Disability"/>
+    <m/>
+    <n v="-1152"/>
+    <s v="SemiMonthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Paycheck"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Healthcare:Premiums"/>
+    <m/>
+    <n v="-6000"/>
+    <s v="SemiMonthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Paycheck"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Savings:401k Match"/>
+    <m/>
+    <n v="-4000"/>
+    <s v="SemiMonthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Paycheck"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Savings:401k Contributions"/>
+    <m/>
+    <n v="-19000"/>
+    <s v="SemiMonthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Paycheck"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Insurance:Life"/>
+    <m/>
+    <n v="-200"/>
+    <s v="SemiMonthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Paycheck"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Insurance:Disability"/>
+    <m/>
+    <n v="-50"/>
+    <s v="SemiMonthly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Paycheck"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Taxes:Federal:Return"/>
+    <s v="IRS"/>
+    <n v="1200"/>
+    <s v="Yearly"/>
+    <s v="None"/>
+    <s v="None"/>
+    <m/>
+    <x v="2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{279950C2-1ED2-47A3-A33A-0974DD3FF0D6}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of AmountYearly" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}" name="Table1" displayName="Table1" ref="A1:G46" totalsRowShown="0">
-  <autoFilter ref="A1:G46" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}" name="Table1" displayName="Table1" ref="A1:H46" totalsRowShown="0">
+  <autoFilter ref="A1:H46" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{2D305D92-F06E-4A42-ADD5-8905CE687361}" name="Category"/>
     <tableColumn id="2" xr3:uid="{CD6746BA-7D2E-459B-9C57-966F0DD88C48}" name="Payee"/>
     <tableColumn id="3" xr3:uid="{93117429-1FD4-4AA7-BE38-B0D0B1C52453}" name="AmountYearly" dataDxfId="0" dataCellStyle="Currency"/>
@@ -415,6 +1879,7 @@
     <tableColumn id="5" xr3:uid="{778F6780-87B7-466A-8305-1DFBFB539DA5}" name="AmountJitter"/>
     <tableColumn id="6" xr3:uid="{57ACD242-AF26-46E4-AC6D-23DE7A7410EC}" name="DateJitter"/>
     <tableColumn id="15" xr3:uid="{A48EA1D1-3BF2-427F-B68E-F650AE4C5A46}" name="Group"/>
+    <tableColumn id="7" xr3:uid="{0CB4C16B-4D70-4E5B-AF7A-7B77AF66D670}" name="Classification"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -717,10 +2182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFC0386-6A87-4615-9CF7-243BB5DCA6C5}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -733,7 +2198,7 @@
     <col min="6" max="7" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -755,8 +2220,11 @@
       <c r="G1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -779,8 +2247,11 @@
       <c r="G2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -800,8 +2271,11 @@
       <c r="G3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -821,8 +2295,11 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -842,8 +2319,11 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -863,8 +2343,11 @@
       <c r="F6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -884,8 +2367,11 @@
       <c r="F7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -904,8 +2390,11 @@
       <c r="F8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -925,8 +2414,11 @@
       <c r="F9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -945,8 +2437,11 @@
       <c r="F10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -965,8 +2460,11 @@
       <c r="F11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -986,8 +2484,11 @@
       <c r="F12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1007,8 +2508,11 @@
       <c r="F13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1028,8 +2532,11 @@
       <c r="F14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1049,8 +2556,11 @@
       <c r="F15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -1070,8 +2580,11 @@
       <c r="F16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -1091,8 +2604,11 @@
       <c r="F17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1112,8 +2628,11 @@
       <c r="F18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1133,8 +2652,11 @@
       <c r="F19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1154,8 +2676,11 @@
       <c r="F20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1175,8 +2700,11 @@
       <c r="F21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1196,8 +2724,11 @@
       <c r="F22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -1217,8 +2748,11 @@
       <c r="F23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1238,8 +2772,11 @@
       <c r="F24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1259,8 +2796,11 @@
       <c r="F25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1280,8 +2820,11 @@
       <c r="F26" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1301,8 +2844,11 @@
       <c r="F27" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1322,8 +2868,11 @@
       <c r="F28" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1343,8 +2892,11 @@
       <c r="F29" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1364,8 +2916,11 @@
       <c r="F30" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1385,8 +2940,11 @@
       <c r="F31" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1406,8 +2964,11 @@
       <c r="F32" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1426,8 +2987,11 @@
       <c r="F33" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1449,8 +3013,11 @@
       <c r="G34" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1470,8 +3037,11 @@
       <c r="G35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1491,8 +3061,11 @@
       <c r="G36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -1512,8 +3085,11 @@
       <c r="G37" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -1533,8 +3109,11 @@
       <c r="G38" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -1554,8 +3133,11 @@
       <c r="G39" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -1575,8 +3157,11 @@
       <c r="G40" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H40" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -1596,8 +3181,11 @@
       <c r="G41" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -1617,8 +3205,11 @@
       <c r="G42" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>38</v>
       </c>
@@ -1638,8 +3229,11 @@
       <c r="G43" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -1659,8 +3253,11 @@
       <c r="G44" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -1680,8 +3277,11 @@
       <c r="G45" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>41</v>
       </c>
@@ -1700,6 +3300,9 @@
       </c>
       <c r="F46" t="s">
         <v>13</v>
+      </c>
+      <c r="H46" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1707,6 +3310,122 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A675DDD4-322B-43C7-B16E-9DB6F82D3792}">
+  <dimension ref="A3:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="4">
+        <v>-56770</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="4">
+        <v>117128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="4">
+        <v>-23000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="4">
+        <v>-17184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="4">
+        <v>20174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10">
+        <f>GETPIVOTDATA("AmountYearly",$A$3,"Classification","Paycheck")</f>
+        <v>117128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11">
+        <f>-GETPIVOTDATA("AmountYearly",$A$3,"Classification","Need")</f>
+        <v>56770</v>
+      </c>
+      <c r="C11" s="5">
+        <f>B11/B10</f>
+        <v>0.48468342326343827</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12">
+        <f>-GETPIVOTDATA("AmountYearly",$A$3,"Classification","Want")</f>
+        <v>17184</v>
+      </c>
+      <c r="C12" s="5">
+        <f>B12/B10</f>
+        <v>0.14671129021241719</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13">
+        <f>-GETPIVOTDATA("AmountYearly",$A$3,"Classification","Save")+GETPIVOTDATA("AmountYearly",$A$3)</f>
+        <v>43174</v>
+      </c>
+      <c r="C13" s="5">
+        <f>B13/B10</f>
+        <v>0.36860528652414454</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Generator cleanup: Task #1098: Add a multiplier generally
</commit_message>
<xml_diff>
--- a/YoFi.AspNet/Data/FullSampleDataDefinition.xlsx
+++ b/YoFi.AspNet/Data/FullSampleDataDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\jcoliz\Ofx\YoFi.AspNet\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E237FFF-D9DF-4905-846B-4A8895FE1D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F455CD-1741-439D-AEF5-73F1FB6DA79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10110" yWindow="2730" windowWidth="28800" windowHeight="15460" xr2:uid="{D78380F0-A539-4D8B-9BEC-B3C0621EF4A6}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId3"/>
+    <pivotCache cacheId="10" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="102">
   <si>
     <t>Housing:Mortgage Interest</t>
   </si>
@@ -268,9 +268,6 @@
     <t>SemiMonthly</t>
   </si>
   <si>
-    <t>ManyPerWeek</t>
-  </si>
-  <si>
     <t>Food:Away:Dinner</t>
   </si>
   <si>
@@ -344,6 +341,9 @@
   </si>
   <si>
     <t>Net Pay</t>
+  </si>
+  <si>
+    <t>DateRepeats</t>
   </si>
 </sst>
 </file>
@@ -1810,7 +1810,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{279950C2-1ED2-47A3-A33A-0974DD3FF0D6}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{279950C2-1ED2-47A3-A33A-0974DD3FF0D6}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -1869,13 +1869,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}" name="Table1" displayName="Table1" ref="A1:H46" totalsRowShown="0">
-  <autoFilter ref="A1:H46" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}" name="Table1" displayName="Table1" ref="A1:I46" totalsRowShown="0">
+  <autoFilter ref="A1:I46" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2D305D92-F06E-4A42-ADD5-8905CE687361}" name="Category"/>
     <tableColumn id="2" xr3:uid="{CD6746BA-7D2E-459B-9C57-966F0DD88C48}" name="Payee"/>
     <tableColumn id="3" xr3:uid="{93117429-1FD4-4AA7-BE38-B0D0B1C52453}" name="AmountYearly" dataDxfId="0" dataCellStyle="Currency"/>
     <tableColumn id="4" xr3:uid="{3579543E-128A-4FB8-8B84-8E3E22C7B7EA}" name="DateFrequency"/>
+    <tableColumn id="8" xr3:uid="{0223E3EB-A5B0-4539-9429-E8AAEE8364AC}" name="DateRepeats"/>
     <tableColumn id="5" xr3:uid="{778F6780-87B7-466A-8305-1DFBFB539DA5}" name="AmountJitter"/>
     <tableColumn id="6" xr3:uid="{57ACD242-AF26-46E4-AC6D-23DE7A7410EC}" name="DateJitter"/>
     <tableColumn id="15" xr3:uid="{A48EA1D1-3BF2-427F-B68E-F650AE4C5A46}" name="Group"/>
@@ -2182,10 +2183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFC0386-6A87-4615-9CF7-243BB5DCA6C5}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2193,12 +2194,13 @@
     <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.08984375" customWidth="1"/>
-    <col min="4" max="4" width="21.6328125" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" customWidth="1"/>
-    <col min="6" max="7" width="11.26953125" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1"/>
+    <col min="7" max="8" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -2206,25 +2208,28 @@
         <v>52</v>
       </c>
       <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
         <v>91</v>
       </c>
-      <c r="D1" t="s">
-        <v>92</v>
-      </c>
       <c r="E1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
         <v>79</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>80</v>
       </c>
-      <c r="G1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -2238,20 +2243,20 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" t="s">
         <v>13</v>
       </c>
       <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
         <v>74</v>
       </c>
-      <c r="H2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2262,25 +2267,25 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" t="s">
         <v>13</v>
       </c>
       <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
         <v>74</v>
       </c>
-      <c r="H3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="1">
         <f>-330*12</f>
@@ -2289,17 +2294,17 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="H4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -2313,22 +2318,22 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
       <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="1">
         <f>-5000</f>
@@ -2337,17 +2342,17 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
       <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
         <v>17</v>
       </c>
-      <c r="H6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2361,22 +2366,22 @@
       <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="H7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="1">
         <v>-800</v>
@@ -2384,22 +2389,22 @@
       <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>15</v>
       </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="1">
         <f>-50*12</f>
@@ -2408,17 +2413,17 @@
       <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>15</v>
       </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -2431,17 +2436,17 @@
       <c r="D10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
       <c r="F10" t="s">
         <v>13</v>
       </c>
-      <c r="H10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2454,17 +2459,17 @@
       <c r="D11" t="s">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
       <c r="F11" t="s">
         <v>13</v>
       </c>
-      <c r="H11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -2478,17 +2483,17 @@
       <c r="D12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
       <c r="F12" t="s">
         <v>13</v>
       </c>
-      <c r="H12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2502,22 +2507,22 @@
       <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
-      <c r="H13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="1">
         <f>-200*12</f>
@@ -2526,22 +2531,22 @@
       <c r="D14" t="s">
         <v>16</v>
       </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
       <c r="F14" t="s">
         <v>17</v>
       </c>
-      <c r="H14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" s="1">
         <f>-85*52</f>
@@ -2550,65 +2555,71 @@
       <c r="D15" t="s">
         <v>16</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>14</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>15</v>
       </c>
-      <c r="H15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1">
         <f>-52*3*7.5</f>
         <v>-1170</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
       </c>
-      <c r="H16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="1">
         <f>-52*3*50</f>
         <v>-7800</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
       </c>
       <c r="F17" t="s">
         <v>17</v>
       </c>
-      <c r="H17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2622,17 +2633,17 @@
       <c r="D18" t="s">
         <v>12</v>
       </c>
-      <c r="E18" t="s">
-        <v>17</v>
-      </c>
       <c r="F18" t="s">
         <v>17</v>
       </c>
-      <c r="H18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2646,17 +2657,17 @@
       <c r="D19" t="s">
         <v>12</v>
       </c>
-      <c r="E19" t="s">
-        <v>17</v>
-      </c>
       <c r="F19" t="s">
         <v>17</v>
       </c>
-      <c r="H19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -2670,17 +2681,17 @@
       <c r="D20" t="s">
         <v>16</v>
       </c>
-      <c r="E20" t="s">
-        <v>17</v>
-      </c>
       <c r="F20" t="s">
         <v>17</v>
       </c>
-      <c r="H20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -2694,17 +2705,17 @@
       <c r="D21" t="s">
         <v>12</v>
       </c>
-      <c r="E21" t="s">
-        <v>13</v>
-      </c>
       <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
         <v>14</v>
       </c>
-      <c r="H21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -2718,17 +2729,17 @@
       <c r="D22" t="s">
         <v>10</v>
       </c>
-      <c r="E22" t="s">
-        <v>17</v>
-      </c>
       <c r="F22" t="s">
         <v>17</v>
       </c>
-      <c r="H22" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -2742,17 +2753,17 @@
       <c r="D23" t="s">
         <v>16</v>
       </c>
-      <c r="E23" t="s">
-        <v>17</v>
-      </c>
       <c r="F23" t="s">
         <v>17</v>
       </c>
-      <c r="H23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2766,17 +2777,17 @@
       <c r="D24" t="s">
         <v>16</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>17</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>14</v>
       </c>
-      <c r="H24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2790,17 +2801,17 @@
       <c r="D25" t="s">
         <v>12</v>
       </c>
-      <c r="E25" t="s">
-        <v>13</v>
-      </c>
       <c r="F25" t="s">
         <v>13</v>
       </c>
-      <c r="H25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -2814,17 +2825,17 @@
       <c r="D26" t="s">
         <v>11</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>15</v>
       </c>
-      <c r="F26" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2838,22 +2849,22 @@
       <c r="D27" t="s">
         <v>10</v>
       </c>
-      <c r="E27" t="s">
-        <v>13</v>
-      </c>
       <c r="F27" t="s">
         <v>13</v>
       </c>
-      <c r="H27" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28" s="1">
         <f>-2000</f>
@@ -2862,17 +2873,17 @@
       <c r="D28" t="s">
         <v>12</v>
       </c>
-      <c r="E28" t="s">
-        <v>17</v>
-      </c>
       <c r="F28" t="s">
         <v>17</v>
       </c>
-      <c r="H28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2886,17 +2897,17 @@
       <c r="D29" t="s">
         <v>10</v>
       </c>
-      <c r="E29" t="s">
-        <v>13</v>
-      </c>
       <c r="F29" t="s">
         <v>13</v>
       </c>
-      <c r="H29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2910,17 +2921,17 @@
       <c r="D30" t="s">
         <v>10</v>
       </c>
-      <c r="E30" t="s">
-        <v>13</v>
-      </c>
       <c r="F30" t="s">
         <v>13</v>
       </c>
-      <c r="H30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G30" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2934,22 +2945,22 @@
       <c r="D31" t="s">
         <v>10</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>15</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>17</v>
       </c>
-      <c r="H31" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" s="1">
         <f>-125*4</f>
@@ -2958,22 +2969,22 @@
       <c r="D32" t="s">
         <v>12</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>15</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>14</v>
       </c>
-      <c r="H32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C33" s="1">
         <v>25000</v>
@@ -2981,22 +2992,22 @@
       <c r="D33" t="s">
         <v>11</v>
       </c>
-      <c r="E33" t="s">
-        <v>13</v>
-      </c>
       <c r="F33" t="s">
         <v>13</v>
       </c>
-      <c r="H33" t="s">
+      <c r="G33" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C34" s="1">
         <v>120000</v>
@@ -3004,20 +3015,20 @@
       <c r="D34" t="s">
         <v>75</v>
       </c>
-      <c r="E34" t="s">
-        <v>13</v>
-      </c>
       <c r="F34" t="s">
         <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="H34" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -3028,20 +3039,20 @@
       <c r="D35" t="s">
         <v>75</v>
       </c>
-      <c r="E35" t="s">
-        <v>13</v>
-      </c>
       <c r="F35" t="s">
         <v>13</v>
       </c>
       <c r="G35" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="H35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -3052,20 +3063,20 @@
       <c r="D36" t="s">
         <v>75</v>
       </c>
-      <c r="E36" t="s">
-        <v>13</v>
-      </c>
       <c r="F36" t="s">
         <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="H36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -3076,20 +3087,20 @@
       <c r="D37" t="s">
         <v>75</v>
       </c>
-      <c r="E37" t="s">
-        <v>13</v>
-      </c>
       <c r="F37" t="s">
         <v>13</v>
       </c>
       <c r="G37" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="H37" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -3100,20 +3111,20 @@
       <c r="D38" t="s">
         <v>75</v>
       </c>
-      <c r="E38" t="s">
-        <v>13</v>
-      </c>
       <c r="F38" t="s">
         <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="H38" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -3124,20 +3135,20 @@
       <c r="D39" t="s">
         <v>75</v>
       </c>
-      <c r="E39" t="s">
-        <v>13</v>
-      </c>
       <c r="F39" t="s">
         <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="H39" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -3148,20 +3159,20 @@
       <c r="D40" t="s">
         <v>75</v>
       </c>
-      <c r="E40" t="s">
-        <v>13</v>
-      </c>
       <c r="F40" t="s">
         <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="H40" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I40" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -3172,20 +3183,20 @@
       <c r="D41" t="s">
         <v>75</v>
       </c>
-      <c r="E41" t="s">
-        <v>13</v>
-      </c>
       <c r="F41" t="s">
         <v>13</v>
       </c>
       <c r="G41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" t="s">
         <v>35</v>
       </c>
-      <c r="H41" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -3196,20 +3207,20 @@
       <c r="D42" t="s">
         <v>75</v>
       </c>
-      <c r="E42" t="s">
-        <v>13</v>
-      </c>
       <c r="F42" t="s">
         <v>13</v>
       </c>
       <c r="G42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" t="s">
         <v>35</v>
       </c>
-      <c r="H42" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>38</v>
       </c>
@@ -3220,20 +3231,20 @@
       <c r="D43" t="s">
         <v>75</v>
       </c>
-      <c r="E43" t="s">
-        <v>13</v>
-      </c>
       <c r="F43" t="s">
         <v>13</v>
       </c>
       <c r="G43" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" t="s">
         <v>35</v>
       </c>
-      <c r="H43" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I43" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -3244,20 +3255,20 @@
       <c r="D44" t="s">
         <v>75</v>
       </c>
-      <c r="E44" t="s">
-        <v>13</v>
-      </c>
       <c r="F44" t="s">
         <v>13</v>
       </c>
       <c r="G44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" t="s">
         <v>35</v>
       </c>
-      <c r="H44" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -3268,20 +3279,20 @@
       <c r="D45" t="s">
         <v>75</v>
       </c>
-      <c r="E45" t="s">
-        <v>13</v>
-      </c>
       <c r="F45" t="s">
         <v>13</v>
       </c>
       <c r="G45" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" t="s">
         <v>35</v>
       </c>
-      <c r="H45" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>41</v>
       </c>
@@ -3295,13 +3306,13 @@
       <c r="D46" t="s">
         <v>11</v>
       </c>
-      <c r="E46" t="s">
-        <v>13</v>
-      </c>
       <c r="F46" t="s">
         <v>13</v>
       </c>
-      <c r="H46" t="s">
+      <c r="G46" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3329,15 +3340,15 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="4">
         <v>-56770</v>
@@ -3353,7 +3364,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" s="4">
         <v>-23000</v>
@@ -3361,7 +3372,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="4">
         <v>-17184</v>
@@ -3369,7 +3380,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="4">
         <v>20174</v>
@@ -3377,7 +3388,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10">
         <f>GETPIVOTDATA("AmountYearly",$A$3,"Classification","Paycheck")</f>
@@ -3386,7 +3397,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11">
         <f>-GETPIVOTDATA("AmountYearly",$A$3,"Classification","Need")</f>
@@ -3399,7 +3410,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12">
         <f>-GETPIVOTDATA("AmountYearly",$A$3,"Classification","Want")</f>
@@ -3412,7 +3423,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13">
         <f>-GETPIVOTDATA("AmountYearly",$A$3,"Classification","Save")+GETPIVOTDATA("AmountYearly",$A$3)</f>

</xml_diff>

<commit_message>
Task #1097: Move some food away budget to lunches out
</commit_message>
<xml_diff>
--- a/YoFi.AspNet/Data/FullSampleDataDefinition.xlsx
+++ b/YoFi.AspNet/Data/FullSampleDataDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\jcoliz\Ofx\YoFi.AspNet\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F455CD-1741-439D-AEF5-73F1FB6DA79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491EF2F6-7800-42D4-BB19-8677500F9D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10110" yWindow="2730" windowWidth="28800" windowHeight="15460" xr2:uid="{D78380F0-A539-4D8B-9BEC-B3C0621EF4A6}"/>
+    <workbookView xWindow="13400" yWindow="5750" windowWidth="28800" windowHeight="15460" xr2:uid="{D78380F0-A539-4D8B-9BEC-B3C0621EF4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleDataPattern" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId3"/>
+    <pivotCache cacheId="3" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="104">
   <si>
     <t>Housing:Mortgage Interest</t>
   </si>
@@ -344,6 +344,12 @@
   </si>
   <si>
     <t>DateRepeats</t>
+  </si>
+  <si>
+    <t>Food:Away:Lunch</t>
+  </si>
+  <si>
+    <t>Qdoba,Chipotle,Subway,Jimmy Johns</t>
   </si>
 </sst>
 </file>
@@ -1810,7 +1816,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{279950C2-1ED2-47A3-A33A-0974DD3FF0D6}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{279950C2-1ED2-47A3-A33A-0974DD3FF0D6}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -1869,8 +1875,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}" name="Table1" displayName="Table1" ref="A1:I46" totalsRowShown="0">
-  <autoFilter ref="A1:I46" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}" name="Table1" displayName="Table1" ref="A1:I47" totalsRowShown="0">
+  <autoFilter ref="A1:I47" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2D305D92-F06E-4A42-ADD5-8905CE687361}" name="Category"/>
     <tableColumn id="2" xr3:uid="{CD6746BA-7D2E-459B-9C57-966F0DD88C48}" name="Payee"/>
@@ -2183,10 +2189,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFC0386-6A87-4615-9CF7-243BB5DCA6C5}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2600,14 +2606,14 @@
         <v>81</v>
       </c>
       <c r="C17" s="1">
-        <f>-52*3*50</f>
+        <f>-52*2*75</f>
         <v>-7800</v>
       </c>
       <c r="D17" t="s">
         <v>16</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="s">
         <v>17</v>
@@ -2621,408 +2627,409 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="1">
+        <f>-52*3*15</f>
+        <v>-2340</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C19" s="1">
         <f>-400</f>
         <v>-400</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>12</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>17</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>17</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I19" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C20" s="1">
         <f>-1200</f>
         <v>-1200</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>12</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>17</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>17</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>47</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C21" s="1">
         <f>-150*12</f>
         <v>-1800</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>16</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" t="s">
         <v>17</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>17</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I21" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>48</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C22" s="1">
         <f>-40*6</f>
         <v>-240</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>12</v>
       </c>
-      <c r="F21" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
         <v>14</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I22" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>50</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C23" s="1">
         <f>-250</f>
         <v>-250</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>10</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
         <v>17</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" t="s">
         <v>17</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I23" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>49</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C24" s="1">
         <f>-200*12</f>
         <v>-2400</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>16</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>17</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G24" t="s">
         <v>17</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C25" s="1">
         <f>52*-35</f>
         <v>-1820</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>16</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F25" t="s">
         <v>17</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G25" t="s">
         <v>14</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C26" s="1">
         <f>-500</f>
         <v>-500</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>12</v>
       </c>
-      <c r="F25" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>43</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C27" s="1">
         <f>-300</f>
         <v>-300</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>11</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>15</v>
       </c>
-      <c r="G26" t="s">
-        <v>13</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C28" s="1">
         <f>-400*12</f>
         <v>-4800</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>10</v>
       </c>
-      <c r="F27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>89</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C29" s="1">
         <f>-2000</f>
         <v>-2000</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>12</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>17</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>17</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I29" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C30" s="1">
         <f>-12*12</f>
         <v>-144</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>10</v>
       </c>
-      <c r="F29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" t="s">
-        <v>13</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="F30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C31" s="1">
         <f>-15*12</f>
         <v>-180</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>10</v>
       </c>
-      <c r="F30" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" t="s">
-        <v>13</v>
-      </c>
-      <c r="I30" t="s">
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C32" s="1">
         <f>-25*12</f>
         <v>-300</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>10</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>15</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G32" t="s">
         <v>17</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I32" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C33" s="1">
         <f>-125*4</f>
         <v>-500</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>12</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>15</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G33" t="s">
         <v>14</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I33" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="1">
-        <v>25000</v>
-      </c>
-      <c r="D33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I33" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
         <v>88</v>
       </c>
       <c r="C34" s="1">
-        <v>120000</v>
+        <v>25000</v>
       </c>
       <c r="D34" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="F34" t="s">
         <v>13</v>
       </c>
       <c r="G34" t="s">
         <v>13</v>
-      </c>
-      <c r="H34" t="s">
-        <v>35</v>
       </c>
       <c r="I34" t="s">
         <v>35</v>
@@ -3030,289 +3037,315 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="1">
+        <v>120000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" t="s">
+        <v>35</v>
+      </c>
+      <c r="I35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C36" s="1">
         <f>4000</f>
         <v>4000</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>75</v>
       </c>
-      <c r="F35" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" t="s">
         <v>35</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C37" s="1">
         <f>-687*24</f>
         <v>-16488</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>75</v>
       </c>
-      <c r="F36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" t="s">
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" t="s">
         <v>35</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C38" s="1">
         <f>-310*24</f>
         <v>-7440</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>75</v>
       </c>
-      <c r="F37" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="F38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" t="s">
         <v>35</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C39" s="1">
         <f>-73*24</f>
         <v>-1752</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>75</v>
       </c>
-      <c r="F38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" t="s">
-        <v>13</v>
-      </c>
-      <c r="H38" t="s">
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" t="s">
         <v>35</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I39" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C40" s="1">
         <f>-260*24</f>
         <v>-6240</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>75</v>
       </c>
-      <c r="F39" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" t="s">
+      <c r="F40" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" t="s">
         <v>35</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I40" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C41" s="1">
         <f>-48*24</f>
         <v>-1152</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>75</v>
       </c>
-      <c r="F40" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="F41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" t="s">
         <v>35</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C42" s="1">
         <f>-500*12</f>
         <v>-6000</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>75</v>
       </c>
-      <c r="F41" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" t="s">
+      <c r="F42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" t="s">
         <v>35</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I42" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C43" s="1">
         <f>-4000</f>
         <v>-4000</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>75</v>
       </c>
-      <c r="F42" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" t="s">
+      <c r="F43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" t="s">
         <v>35</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I43" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C44" s="1">
         <f>-19000</f>
         <v>-19000</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>75</v>
       </c>
-      <c r="F43" t="s">
-        <v>13</v>
-      </c>
-      <c r="G43" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" t="s">
+      <c r="F44" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" t="s">
         <v>35</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I44" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C45" s="1">
         <f>-200</f>
         <v>-200</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>75</v>
       </c>
-      <c r="F44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" t="s">
-        <v>13</v>
-      </c>
-      <c r="H44" t="s">
+      <c r="F45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" t="s">
         <v>35</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I45" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C46" s="1">
         <f>-50</f>
         <v>-50</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>75</v>
       </c>
-      <c r="F45" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" t="s">
-        <v>13</v>
-      </c>
-      <c r="H45" t="s">
+      <c r="F46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" t="s">
         <v>35</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I46" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>41</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C47" s="1">
         <f>1200</f>
         <v>1200</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>11</v>
       </c>
-      <c r="F46" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" t="s">
-        <v>13</v>
-      </c>
-      <c r="I46" t="s">
+      <c r="F47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished Task #1199: Add auto loan calculation to sample data, including the data itself. Yikes, a lot of change
</commit_message>
<xml_diff>
--- a/YoFi.AspNet/Data/FullSampleDataDefinition.xlsx
+++ b/YoFi.AspNet/Data/FullSampleDataDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\jcoliz\Ofx\YoFi.AspNet\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491EF2F6-7800-42D4-BB19-8677500F9D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B52952E-2670-4BE9-B9B2-B762FA5FCA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13400" yWindow="5750" windowWidth="28800" windowHeight="15460" xr2:uid="{D78380F0-A539-4D8B-9BEC-B3C0621EF4A6}"/>
+    <workbookView xWindow="9040" yWindow="4060" windowWidth="24420" windowHeight="15460" xr2:uid="{D78380F0-A539-4D8B-9BEC-B3C0621EF4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleDataPattern" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="104">
-  <si>
-    <t>Housing:Mortgage Interest</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="105">
   <si>
     <t>Housing:Property Tax</t>
   </si>
@@ -350,6 +347,12 @@
   </si>
   <si>
     <t>Qdoba,Chipotle,Subway,Jimmy Johns</t>
+  </si>
+  <si>
+    <t>Loan</t>
+  </si>
+  <si>
+    <t>{ "interest": "Housing:Mortgage Interest", "amount": 375000, "rate": 3, "term": 360, "origination": "1/1/2010" }</t>
   </si>
 </sst>
 </file>
@@ -1816,7 +1819,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{279950C2-1ED2-47A3-A33A-0974DD3FF0D6}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{279950C2-1ED2-47A3-A33A-0974DD3FF0D6}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -1875,9 +1878,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}" name="Table1" displayName="Table1" ref="A1:I47" totalsRowShown="0">
-  <autoFilter ref="A1:I47" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}" name="Table1" displayName="Table1" ref="A1:J46" totalsRowShown="0">
+  <autoFilter ref="A1:J46" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{2D305D92-F06E-4A42-ADD5-8905CE687361}" name="Category"/>
     <tableColumn id="2" xr3:uid="{CD6746BA-7D2E-459B-9C57-966F0DD88C48}" name="Payee"/>
     <tableColumn id="3" xr3:uid="{93117429-1FD4-4AA7-BE38-B0D0B1C52453}" name="AmountYearly" dataDxfId="0" dataCellStyle="Currency"/>
@@ -1887,6 +1890,7 @@
     <tableColumn id="6" xr3:uid="{57ACD242-AF26-46E4-AC6D-23DE7A7410EC}" name="DateJitter"/>
     <tableColumn id="15" xr3:uid="{A48EA1D1-3BF2-427F-B68E-F650AE4C5A46}" name="Group"/>
     <tableColumn id="7" xr3:uid="{0CB4C16B-4D70-4E5B-AF7A-7B77AF66D670}" name="Classification"/>
+    <tableColumn id="9" xr3:uid="{B6795423-1DFB-40DC-BB3C-6D6DCA420B25}" name="Loan"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2189,10 +2193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFC0386-6A87-4615-9CF7-243BB5DCA6C5}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2206,450 +2210,456 @@
     <col min="7" max="8" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
       <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" t="s">
         <v>90</v>
       </c>
-      <c r="D1" t="s">
-        <v>91</v>
-      </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
         <v>78</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" t="s">
-        <v>80</v>
-      </c>
       <c r="I1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1">
         <f>-800*12</f>
         <v>-9600</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+      <c r="J2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
       </c>
       <c r="C3" s="1">
-        <f>-700*12</f>
-        <v>-8400</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="1">
         <f>-330*12</f>
         <v>-3960</v>
       </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="1">
+        <f>-400</f>
+        <v>-400</v>
+      </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="1">
+        <f>-5000</f>
+        <v>-5000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="1">
+        <f>-300*12</f>
+        <v>-3600</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-800</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="1">
+        <f>-50*12</f>
+        <v>-600</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-700</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-400</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="1">
+        <f>-95*12</f>
+        <v>-1140</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="1">
+        <f>-40*12</f>
+        <v>-480</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="1">
+        <f>-200*12</f>
+        <v>-2400</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="1">
+        <f>-85*52</f>
+        <v>-4420</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
         <v>13</v>
       </c>
-      <c r="I4" t="s">
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="1">
+        <f>-52*3*7.5</f>
+        <v>-1170</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="1">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="1">
+        <f>-52*2*75</f>
+        <v>-7800</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="1">
+        <f>-52*3*15</f>
+        <v>-2340</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="1">
         <f>-400</f>
         <v>-400</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D18" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="1">
-        <f>-5000</f>
-        <v>-5000</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="1">
-        <f>-300*12</f>
-        <v>-3600</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="1">
-        <v>-800</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="1">
-        <f>-50*12</f>
-        <v>-600</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="1">
-        <v>-700</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="1">
-        <v>-400</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="1">
-        <f>-95*12</f>
-        <v>-1140</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="1">
-        <f>-40*12</f>
-        <v>-480</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="1">
-        <f>-200*12</f>
-        <v>-2400</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="F18" t="s">
         <v>16</v>
       </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="1">
-        <f>-85*52</f>
-        <v>-4420</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="G18" t="s">
         <v>16</v>
       </c>
-      <c r="F15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="1">
-        <f>-52*3*7.5</f>
-        <v>-1170</v>
-      </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
-      </c>
-      <c r="F16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="1">
-        <f>-52*2*75</f>
-        <v>-7800</v>
-      </c>
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>102</v>
-      </c>
-      <c r="B18" t="s">
-        <v>103</v>
-      </c>
-      <c r="C18" s="1">
-        <f>-52*3*15</f>
-        <v>-2340</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18">
-        <v>3</v>
-      </c>
-      <c r="F18" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" t="s">
-        <v>17</v>
-      </c>
       <c r="I18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -2657,44 +2667,44 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="1">
-        <f>-400</f>
-        <v>-400</v>
+        <f>-1200</f>
+        <v>-1200</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C20" s="1">
-        <f>-1200</f>
-        <v>-1200</v>
+        <f>-150*12</f>
+        <v>-1800</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I20" t="s">
         <v>94</v>
@@ -2705,95 +2715,95 @@
         <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21" s="1">
-        <f>-150*12</f>
-        <v>-1800</v>
+        <f>-40*6</f>
+        <v>-240</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22" s="1">
-        <f>-40*6</f>
-        <v>-240</v>
+        <f>-250</f>
+        <v>-250</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C23" s="1">
-        <f>-250</f>
-        <v>-250</v>
+        <f>-200*12</f>
+        <v>-2400</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C24" s="1">
-        <f>-200*12</f>
-        <v>-2400</v>
+        <f>52*-35</f>
+        <v>-1820</v>
       </c>
       <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" t="s">
         <v>16</v>
       </c>
-      <c r="F24" t="s">
-        <v>17</v>
-      </c>
       <c r="G24" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -2801,71 +2811,71 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C25" s="1">
-        <f>52*-35</f>
-        <v>-1820</v>
+        <f>-500</f>
+        <v>-500</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C26" s="1">
-        <f>-500</f>
-        <v>-500</v>
+        <f>-300</f>
+        <v>-300</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
         <v>64</v>
       </c>
       <c r="C27" s="1">
-        <f>-300</f>
-        <v>-300</v>
+        <f>-400*12</f>
+        <v>-4800</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -2873,44 +2883,44 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="C28" s="1">
-        <f>-400*12</f>
-        <v>-4800</v>
+        <f>-2000</f>
+        <v>-2000</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G28" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="C29" s="1">
-        <f>-2000</f>
-        <v>-2000</v>
+        <f>-12*12</f>
+        <v>-144</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I29" t="s">
         <v>94</v>
@@ -2921,23 +2931,23 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C30" s="1">
-        <f>-12*12</f>
-        <v>-144</v>
+        <f>-15*12</f>
+        <v>-180</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
@@ -2948,20 +2958,20 @@
         <v>60</v>
       </c>
       <c r="C31" s="1">
-        <f>-15*12</f>
-        <v>-180</v>
+        <f>-25*12</f>
+        <v>-300</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G31" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
@@ -2969,144 +2979,144 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="C32" s="1">
-        <f>-25*12</f>
-        <v>-300</v>
+        <f>-125*4</f>
+        <v>-500</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G32" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
         <v>87</v>
       </c>
       <c r="C33" s="1">
-        <f>-125*4</f>
-        <v>-500</v>
+        <v>25000</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I33" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C34" s="1">
-        <v>25000</v>
+        <v>120000</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="F34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="H34" t="s">
+        <v>34</v>
       </c>
       <c r="I34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C35" s="1">
-        <v>120000</v>
+        <f>4000</f>
+        <v>4000</v>
       </c>
       <c r="D35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C36" s="1">
-        <f>4000</f>
-        <v>4000</v>
+        <f>-687*24</f>
+        <v>-16488</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C37" s="1">
-        <f>-687*24</f>
-        <v>-16488</v>
+        <f>-310*24</f>
+        <v>-7440</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -3114,47 +3124,47 @@
         <v>33</v>
       </c>
       <c r="C38" s="1">
-        <f>-310*24</f>
-        <v>-7440</v>
+        <f>-73*24</f>
+        <v>-1752</v>
       </c>
       <c r="D38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="1">
+        <f>-260*24</f>
+        <v>-6240</v>
+      </c>
+      <c r="D39" t="s">
+        <v>74</v>
+      </c>
+      <c r="F39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="1">
-        <f>-73*24</f>
-        <v>-1752</v>
-      </c>
-      <c r="D39" t="s">
-        <v>75</v>
-      </c>
-      <c r="F39" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" t="s">
-        <v>35</v>
-      </c>
       <c r="I39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -3162,71 +3172,71 @@
         <v>45</v>
       </c>
       <c r="C40" s="1">
-        <f>-260*24</f>
-        <v>-6240</v>
+        <f>-48*24</f>
+        <v>-1152</v>
       </c>
       <c r="D40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="C41" s="1">
-        <f>-48*24</f>
-        <v>-1152</v>
+        <f>-500*12</f>
+        <v>-6000</v>
       </c>
       <c r="D41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I41" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C42" s="1">
-        <f>-500*12</f>
-        <v>-6000</v>
+        <f>-4000</f>
+        <v>-4000</v>
       </c>
       <c r="D42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I42" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -3234,47 +3244,47 @@
         <v>37</v>
       </c>
       <c r="C43" s="1">
-        <f>-4000</f>
-        <v>-4000</v>
+        <f>-19000</f>
+        <v>-19000</v>
       </c>
       <c r="D43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C44" s="1">
-        <f>-19000</f>
-        <v>-19000</v>
+        <f>-200</f>
+        <v>-200</v>
       </c>
       <c r="D44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I44" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -3282,71 +3292,47 @@
         <v>21</v>
       </c>
       <c r="C45" s="1">
-        <f>-200</f>
-        <v>-200</v>
+        <f>-50</f>
+        <v>-50</v>
       </c>
       <c r="D45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>22</v>
+        <v>40</v>
+      </c>
+      <c r="B46" t="s">
+        <v>66</v>
       </c>
       <c r="C46" s="1">
-        <f>-50</f>
-        <v>-50</v>
-      </c>
-      <c r="D46" t="s">
-        <v>75</v>
-      </c>
-      <c r="F46" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" t="s">
-        <v>13</v>
-      </c>
-      <c r="H46" t="s">
-        <v>35</v>
-      </c>
-      <c r="I46" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>41</v>
-      </c>
-      <c r="B47" t="s">
-        <v>67</v>
-      </c>
-      <c r="C47" s="1">
         <f>1200</f>
         <v>1200</v>
       </c>
-      <c r="D47" t="s">
-        <v>11</v>
-      </c>
-      <c r="F47" t="s">
-        <v>13</v>
-      </c>
-      <c r="G47" t="s">
-        <v>13</v>
-      </c>
-      <c r="I47" t="s">
-        <v>35</v>
+      <c r="D46" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3373,15 +3359,15 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="4">
         <v>-56770</v>
@@ -3389,7 +3375,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="4">
         <v>117128</v>
@@ -3397,7 +3383,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="4">
         <v>-23000</v>
@@ -3405,7 +3391,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="4">
         <v>-17184</v>
@@ -3413,7 +3399,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" s="4">
         <v>20174</v>
@@ -3421,7 +3407,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10">
         <f>GETPIVOTDATA("AmountYearly",$A$3,"Classification","Paycheck")</f>
@@ -3430,7 +3416,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11">
         <f>-GETPIVOTDATA("AmountYearly",$A$3,"Classification","Need")</f>
@@ -3443,7 +3429,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12">
         <f>-GETPIVOTDATA("AmountYearly",$A$3,"Classification","Want")</f>
@@ -3456,7 +3442,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13">
         <f>-GETPIVOTDATA("AmountYearly",$A$3,"Classification","Save")+GETPIVOTDATA("AmountYearly",$A$3)</f>

</xml_diff>